<commit_message>
Add always-on tags for building buttons
</commit_message>
<xml_diff>
--- a/External/Color.xlsx
+++ b/External/Color.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\.EECS494.game_design\20230418\External\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E162CBD4-7EF9-4683-8AA6-6D0DA9EDADE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0DAF82-4395-4498-B230-80C781CC1562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15800" xr2:uid="{F3BD655C-4B5A-43F3-A13D-CB6269306AAB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Mbig</t>
   </si>
@@ -114,6 +114,10 @@
   </si>
   <si>
     <t>Building</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>569eda</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -676,7 +680,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" t="s">

</xml_diff>